<commit_message>
Before Class Week 2
</commit_message>
<xml_diff>
--- a/data/ClassData.xlsx
+++ b/data/ClassData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\courses\qmsa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93F274F-4A02-4D59-84F4-8C00F6BCD3D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C3E78C-AAC7-489B-AEC0-8EFA6666DE4C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{2FCD6EFA-A2DB-4D92-B665-54BD2494A43F}"/>
   </bookViews>
   <sheets>
-    <sheet name="4.4" sheetId="1" r:id="rId1"/>
+    <sheet name="3.1" sheetId="2" r:id="rId1"/>
+    <sheet name="4.4" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Point</t>
   </si>
@@ -64,6 +65,9 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>Precip</t>
   </si>
 </sst>
 </file>
@@ -414,10 +418,230 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FAA05C8-3F86-4BDF-B35B-9228FEC07557}">
+  <dimension ref="A1:A41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>26.87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>26.94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>28.28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>29.48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>31.56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>32.78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>33.07</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>33.619999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>34.979999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>35.090000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>35.200000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>35.380000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>35.96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>36.020000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>36.65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>36.83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>36.99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>38.15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>39.340000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>39.619999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>39.86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>40.21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>40.54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>41.11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>41.34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>41.44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>41.94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>43.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>43.53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>45.62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>46.02</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
+        <v>47.73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
+        <v>47.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>48.02</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>50.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>51.17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>51.97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>54.29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>57.54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2CB7B41-D33A-4AB5-8ACD-EE9F59B5B538}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
After Class Week 2
</commit_message>
<xml_diff>
--- a/data/ClassData.xlsx
+++ b/data/ClassData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\courses\qmsa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C3E78C-AAC7-489B-AEC0-8EFA6666DE4C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51772BD-FF97-415C-8056-636B6095B0C1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{2FCD6EFA-A2DB-4D92-B665-54BD2494A43F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Point</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Precip</t>
+  </si>
+  <si>
+    <t>Precip_cm</t>
   </si>
 </sst>
 </file>
@@ -419,217 +422,380 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FAA05C8-3F86-4BDF-B35B-9228FEC07557}">
-  <dimension ref="A1:A41"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>26.87</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2">
+        <f>A2*2.54</f>
+        <v>68.249800000000008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>26.94</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3">
+        <f t="shared" ref="B3:B41" si="0">A3*2.54</f>
+        <v>68.427599999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>28.28</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>71.83120000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>29.48</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>74.879199999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>31.56</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>80.162399999999991</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>32.78</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>83.261200000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>33.07</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>83.997799999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>33.619999999999997</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>85.394799999999989</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>34.979999999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>88.849199999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>35.090000000000003</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>89.128600000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>35.200000000000003</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>89.408000000000015</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>35.380000000000003</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>89.865200000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>35.96</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>91.338400000000007</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>36.020000000000003</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>91.490800000000007</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>36.65</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>93.090999999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>36.83</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>93.548199999999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>36.99</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>93.954600000000013</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>38.15</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>96.900999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>39.340000000000003</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>99.923600000000008</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>39.619999999999997</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>100.6348</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>39.86</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>101.2444</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>40.21</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>102.13340000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>40.54</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>102.9716</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>41.11</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>104.4194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>41.34</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>105.00360000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>41.44</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>105.2576</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>41.46</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>105.30840000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>41.94</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>106.52759999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>43.3</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>109.982</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>43.53</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>110.56620000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>45.62</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>115.87479999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>46.02</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>116.89080000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>47.73</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>121.23419999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>47.9</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>121.666</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>48.02</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>121.97080000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>50.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>128.27000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <v>51.17</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>129.9718</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>51.97</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>132.00380000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>54.29</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>137.89660000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>57.54</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>146.1516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Before Class Weeks 3
</commit_message>
<xml_diff>
--- a/data/ClassData.xlsx
+++ b/data/ClassData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\courses\qmsa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51772BD-FF97-415C-8056-636B6095B0C1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEA7AAF-0629-44C0-A0A5-F680EB561B50}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{2FCD6EFA-A2DB-4D92-B665-54BD2494A43F}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{2FCD6EFA-A2DB-4D92-B665-54BD2494A43F}"/>
   </bookViews>
   <sheets>
     <sheet name="3.1" sheetId="2" r:id="rId1"/>
     <sheet name="4.4" sheetId="1" r:id="rId2"/>
+    <sheet name="5.1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Point</t>
   </si>
@@ -71,6 +72,42 @@
   </si>
   <si>
     <t>Precip_cm</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Phillippines</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>Totals</t>
   </si>
 </sst>
 </file>
@@ -424,7 +461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FAA05C8-3F86-4BDF-B35B-9228FEC07557}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B41"/>
     </sheetView>
   </sheetViews>
@@ -928,4 +965,180 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B17300-EA79-4141-AF67-3E30BC98C9B6}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>50645</v>
+      </c>
+      <c r="C2">
+        <v>2437</v>
+      </c>
+      <c r="D2">
+        <v>3113</v>
+      </c>
+      <c r="E2">
+        <v>32811</v>
+      </c>
+      <c r="F2">
+        <v>2437</v>
+      </c>
+      <c r="G2">
+        <v>139120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>18680</v>
+      </c>
+      <c r="C3">
+        <v>18859</v>
+      </c>
+      <c r="D3">
+        <v>1620</v>
+      </c>
+      <c r="E3">
+        <v>3280</v>
+      </c>
+      <c r="F3">
+        <v>2253</v>
+      </c>
+      <c r="G3">
+        <v>70863</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>15099</v>
+      </c>
+      <c r="C4">
+        <v>5116</v>
+      </c>
+      <c r="D4">
+        <v>2019</v>
+      </c>
+      <c r="E4">
+        <v>5777</v>
+      </c>
+      <c r="F4">
+        <v>8123</v>
+      </c>
+      <c r="G4">
+        <v>69162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>24082</v>
+      </c>
+      <c r="C5">
+        <v>2361</v>
+      </c>
+      <c r="D5">
+        <v>2320</v>
+      </c>
+      <c r="E5">
+        <v>2525</v>
+      </c>
+      <c r="F5">
+        <v>2321</v>
+      </c>
+      <c r="G5">
+        <v>58173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>172</v>
+      </c>
+      <c r="C6">
+        <v>26249</v>
+      </c>
+      <c r="D6">
+        <v>3900</v>
+      </c>
+      <c r="E6">
+        <v>275</v>
+      </c>
+      <c r="F6">
+        <v>8444</v>
+      </c>
+      <c r="G6">
+        <v>53870</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>208446</v>
+      </c>
+      <c r="C7">
+        <v>147999</v>
+      </c>
+      <c r="D7">
+        <v>107276</v>
+      </c>
+      <c r="E7">
+        <v>87750</v>
+      </c>
+      <c r="F7">
+        <v>56920</v>
+      </c>
+      <c r="G7">
+        <v>1042625</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
before class 4 2
</commit_message>
<xml_diff>
--- a/data/ClassData.xlsx
+++ b/data/ClassData.xlsx
@@ -8,15 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\courses\qmsa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEA7AAF-0629-44C0-A0A5-F680EB561B50}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6E23DD-7560-47A7-80B6-7DBE8C4BA358}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{2FCD6EFA-A2DB-4D92-B665-54BD2494A43F}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{2FCD6EFA-A2DB-4D92-B665-54BD2494A43F}"/>
   </bookViews>
   <sheets>
     <sheet name="3.1" sheetId="2" r:id="rId1"/>
     <sheet name="4.4" sheetId="1" r:id="rId2"/>
     <sheet name="5.1" sheetId="3" r:id="rId3"/>
+    <sheet name="DiscreateProbStarter" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="averageRaber">DiscreateProbStarter!$B$3</definedName>
+    <definedName name="averageRate">DiscreateProbStarter!$B$3</definedName>
+    <definedName name="gstp">DiscreateProbStarter!$H$2</definedName>
+    <definedName name="gt">DiscreateProbStarter!$H$3</definedName>
+    <definedName name="stp">DiscreateProbStarter!$E$2</definedName>
+    <definedName name="trials">DiscreateProbStarter!$E$3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Point</t>
   </si>
@@ -108,14 +117,58 @@
   </si>
   <si>
     <t>Totals</t>
+  </si>
+  <si>
+    <t>Cum_Prob</t>
+  </si>
+  <si>
+    <t>Prob</t>
+  </si>
+  <si>
+    <t>Num of Trials</t>
+  </si>
+  <si>
+    <t>Successes</t>
+  </si>
+  <si>
+    <t>Geometric</t>
+  </si>
+  <si>
+    <t>Binomial</t>
+  </si>
+  <si>
+    <t>Poisson</t>
+  </si>
+  <si>
+    <t>Freq</t>
+  </si>
+  <si>
+    <t>Average Rate</t>
+  </si>
+  <si>
+    <t>SingleTrialProb</t>
+  </si>
+  <si>
+    <t>Trials (Years etc)</t>
+  </si>
+  <si>
+    <t>Single Trial Prob</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -143,8 +196,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -971,7 +1026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B17300-EA79-4141-AF67-3E30BC98C9B6}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -1141,4 +1196,250 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E0F434-671F-4171-9802-12BE55AD7001}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="13.734375" customWidth="1"/>
+    <col min="4" max="4" width="17.3671875" customWidth="1"/>
+    <col min="7" max="7" width="14.1015625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>1.8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <f>_xlfn.POISSON.DIST(A5,averageRaber,FALSE)</f>
+        <v>0.16529888822158653</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f>_xlfn.BINOM.DIST(A5,trials,stp,FALSE)</f>
+        <v>0.41821194239999998</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f>gstp*((1-gstp)^(G5-1))</f>
+        <v>0.16</v>
+      </c>
+      <c r="I5">
+        <f>H5</f>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <f>_xlfn.POISSON.DIST(A6,averageRaber,FALSE)</f>
+        <v>0.29753799879885579</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f>_xlfn.BINOM.DIST(A6,trials,stp,FALSE)</f>
+        <v>0.39829708799999997</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <f>gstp*((1-gstp)^(G6-1))</f>
+        <v>0.13439999999999999</v>
+      </c>
+      <c r="I6">
+        <f>I5+H6</f>
+        <v>0.2944</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <f>_xlfn.POISSON.DIST(A7,averageRaber,FALSE)</f>
+        <v>0.26778419891897026</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <f>_xlfn.BINOM.DIST(A7,trials,stp,FALSE)</f>
+        <v>0.15173222399999997</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <f>gstp*((1-gstp)^(G7-1))</f>
+        <v>0.11289599999999998</v>
+      </c>
+      <c r="I7">
+        <f>I6+H7</f>
+        <v>0.40729599999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <f>_xlfn.POISSON.DIST(A8,averageRaber,FALSE)</f>
+        <v>0.16067051935138213</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <f>_xlfn.BINOM.DIST(A8,trials,stp,FALSE)</f>
+        <v>2.8901375999999999E-2</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <f>gstp*((1-gstp)^(G8-1))</f>
+        <v>9.4832639999999982E-2</v>
+      </c>
+      <c r="I8">
+        <f>I7+H8</f>
+        <v>0.50212864000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <f>_xlfn.POISSON.DIST(A9,averageRaber,FALSE)</f>
+        <v>7.2301733708121985E-2</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <f>_xlfn.BINOM.DIST(A9,trials,stp,FALSE)</f>
+        <v>2.7525120000000025E-3</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <f>gstp*((1-gstp)^(G9-1))</f>
+        <v>7.9659417599999977E-2</v>
+      </c>
+      <c r="I9">
+        <f>I8+H9</f>
+        <v>0.58178805759999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <f>_xlfn.POISSON.DIST(A10,averageRaber,FALSE)</f>
+        <v>2.6028624134923937E-2</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <f>_xlfn.BINOM.DIST(A10,trials,stp,FALSE)</f>
+        <v>1.0485759999999996E-4</v>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+      <c r="H10">
+        <f>gstp*((1-gstp)^(G10-1))</f>
+        <v>6.6913910783999983E-2</v>
+      </c>
+      <c r="I10">
+        <f>I9+H10</f>
+        <v>0.64870196838399996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
AFter class Week 4
</commit_message>
<xml_diff>
--- a/data/ClassData.xlsx
+++ b/data/ClassData.xlsx
@@ -8,23 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\courses\qmsa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6E23DD-7560-47A7-80B6-7DBE8C4BA358}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A71E40-9524-4C51-B4E7-E5587694DD9D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{2FCD6EFA-A2DB-4D92-B665-54BD2494A43F}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="5" xr2:uid="{2FCD6EFA-A2DB-4D92-B665-54BD2494A43F}"/>
   </bookViews>
   <sheets>
     <sheet name="3.1" sheetId="2" r:id="rId1"/>
     <sheet name="4.4" sheetId="1" r:id="rId2"/>
     <sheet name="5.1" sheetId="3" r:id="rId3"/>
     <sheet name="DiscreateProbStarter" sheetId="4" r:id="rId4"/>
+    <sheet name="ContinuousProbStarter" sheetId="6" r:id="rId5"/>
+    <sheet name="ContinuousProbStarter (2)" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="averageRaber">DiscreateProbStarter!$B$3</definedName>
     <definedName name="averageRate">DiscreateProbStarter!$B$3</definedName>
-    <definedName name="gstp">DiscreateProbStarter!$H$2</definedName>
-    <definedName name="gt">DiscreateProbStarter!$H$3</definedName>
-    <definedName name="stp">DiscreateProbStarter!$E$2</definedName>
-    <definedName name="trials">DiscreateProbStarter!$E$3</definedName>
+    <definedName name="gstp">DiscreateProbStarter!$J$2</definedName>
+    <definedName name="gt">DiscreateProbStarter!$J$3</definedName>
+    <definedName name="mean" localSheetId="5">'ContinuousProbStarter (2)'!$A$3</definedName>
+    <definedName name="mean">ContinuousProbStarter!$A$3</definedName>
+    <definedName name="std" localSheetId="5">'ContinuousProbStarter (2)'!$A$4</definedName>
+    <definedName name="std">ContinuousProbStarter!$A$4</definedName>
+    <definedName name="stp">DiscreateProbStarter!$F$2</definedName>
+    <definedName name="trials">DiscreateProbStarter!$F$3</definedName>
+    <definedName name="units">DiscreateProbStarter!$C$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>Point</t>
   </si>
@@ -153,6 +160,27 @@
   </si>
   <si>
     <t>Single Trial Prob</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>StandardDiv</t>
+  </si>
+  <si>
+    <t>Test Value</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Normal Find Prob</t>
+  </si>
+  <si>
+    <t>Normal Find Cutoff</t>
+  </si>
+  <si>
+    <t>Answer(Cutoff)</t>
   </si>
 </sst>
 </file>
@@ -1200,246 +1228,695 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E0F434-671F-4171-9802-12BE55AD7001}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="13.734375" customWidth="1"/>
-    <col min="4" max="4" width="17.3671875" customWidth="1"/>
-    <col min="7" max="7" width="14.1015625" customWidth="1"/>
+    <col min="5" max="5" width="17.3671875" customWidth="1"/>
+    <col min="9" max="9" width="14.1015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="D2" s="2" t="s">
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="E2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>0.16</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="2">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J2" s="2">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>33</v>
       </c>
       <c r="B3">
-        <v>1.8</v>
-      </c>
-      <c r="D3" t="s">
+        <v>6.7619049999999996</v>
+      </c>
+      <c r="E3" t="s">
         <v>35</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>26</v>
       </c>
       <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>26</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="B5">
-        <f>_xlfn.POISSON.DIST(A5,averageRaber,FALSE)</f>
-        <v>0.16529888822158653</v>
+        <f t="shared" ref="B5:B25" si="0">_xlfn.POISSON.DIST(A5,averageRaber,FALSE)</f>
+        <v>1.1570229444290839E-3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C25" si="1">units*B5</f>
+        <v>2.4297481833010764E-2</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <f>_xlfn.BINOM.DIST(A5,trials,stp,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F10" si="2">_xlfn.BINOM.DIST(A5,trials,stp,FALSE)</f>
         <v>0.41821194239999998</v>
       </c>
       <c r="G5">
+        <f t="shared" ref="G5:G10" si="3">_xlfn.BINOM.DIST(E5,trials,stp,TRUE)</f>
+        <v>0.41821194239999998</v>
+      </c>
+      <c r="I5">
         <v>1</v>
       </c>
-      <c r="H5">
-        <f>gstp*((1-gstp)^(G5-1))</f>
-        <v>0.16</v>
-      </c>
-      <c r="I5">
-        <f>H5</f>
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J5">
+        <f t="shared" ref="J5:J10" si="4">gstp*((1-gstp)^(I5-1))</f>
+        <v>0.18</v>
+      </c>
+      <c r="K5">
+        <f>J5</f>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6">
-        <f>_xlfn.POISSON.DIST(A6,averageRaber,FALSE)</f>
-        <v>0.29753799879885579</v>
+        <f t="shared" si="0"/>
+        <v>7.8236792330497445E-3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>0.16429726389404464</v>
       </c>
       <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
         <v>1</v>
       </c>
-      <c r="E6">
-        <f>_xlfn.BINOM.DIST(A6,trials,stp,FALSE)</f>
+      <c r="F6">
+        <f t="shared" si="2"/>
         <v>0.39829708799999997</v>
       </c>
       <c r="G6">
+        <f t="shared" si="3"/>
+        <v>0.81650903040000011</v>
+      </c>
+      <c r="I6">
         <v>2</v>
       </c>
-      <c r="H6">
-        <f>gstp*((1-gstp)^(G6-1))</f>
-        <v>0.13439999999999999</v>
-      </c>
-      <c r="I6">
-        <f>I5+H6</f>
-        <v>0.2944</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J6">
+        <f t="shared" si="4"/>
+        <v>0.14760000000000001</v>
+      </c>
+      <c r="K6">
+        <f>K5+J6</f>
+        <v>0.3276</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7">
-        <f>_xlfn.POISSON.DIST(A7,averageRaber,FALSE)</f>
-        <v>0.26778419891897026</v>
+        <f t="shared" si="0"/>
+        <v>2.6451487862177624E-2</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>0.55548124510573005</v>
       </c>
       <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
         <v>2</v>
       </c>
-      <c r="E7">
-        <f>_xlfn.BINOM.DIST(A7,trials,stp,FALSE)</f>
+      <c r="F7">
+        <f t="shared" si="2"/>
         <v>0.15173222399999997</v>
       </c>
       <c r="G7">
+        <f t="shared" si="3"/>
+        <v>0.96824125440000008</v>
+      </c>
+      <c r="I7">
         <v>3</v>
       </c>
-      <c r="H7">
-        <f>gstp*((1-gstp)^(G7-1))</f>
-        <v>0.11289599999999998</v>
-      </c>
-      <c r="I7">
-        <f>I6+H7</f>
-        <v>0.40729599999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J7">
+        <f t="shared" si="4"/>
+        <v>0.12103200000000001</v>
+      </c>
+      <c r="K7">
+        <f>K6+J7</f>
+        <v>0.44863200000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>3</v>
       </c>
       <c r="B8">
-        <f>_xlfn.POISSON.DIST(A8,averageRaber,FALSE)</f>
-        <v>0.16067051935138213</v>
+        <f t="shared" si="0"/>
+        <v>5.9620816010899393E-2</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>1.2520371362288873</v>
       </c>
       <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
         <v>3</v>
       </c>
-      <c r="E8">
-        <f>_xlfn.BINOM.DIST(A8,trials,stp,FALSE)</f>
+      <c r="F8">
+        <f t="shared" si="2"/>
         <v>2.8901375999999999E-2</v>
       </c>
       <c r="G8">
+        <f t="shared" si="3"/>
+        <v>0.99714263039999995</v>
+      </c>
+      <c r="I8">
         <v>4</v>
       </c>
-      <c r="H8">
-        <f>gstp*((1-gstp)^(G8-1))</f>
-        <v>9.4832639999999982E-2</v>
-      </c>
-      <c r="I8">
-        <f>I7+H8</f>
-        <v>0.50212864000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J8">
+        <f t="shared" si="4"/>
+        <v>9.9246240000000013E-2</v>
+      </c>
+      <c r="K8">
+        <f>K7+J8</f>
+        <v>0.54787824000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>4</v>
       </c>
       <c r="B9">
-        <f>_xlfn.POISSON.DIST(A9,averageRaber,FALSE)</f>
-        <v>7.2301733708121985E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.10078757347204516</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>2.1165390429129483</v>
       </c>
       <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
         <v>4</v>
       </c>
-      <c r="E9">
-        <f>_xlfn.BINOM.DIST(A9,trials,stp,FALSE)</f>
+      <c r="F9">
+        <f t="shared" si="2"/>
         <v>2.7525120000000025E-3</v>
       </c>
       <c r="G9">
+        <f t="shared" si="3"/>
+        <v>0.99989514239999999</v>
+      </c>
+      <c r="I9">
         <v>5</v>
       </c>
-      <c r="H9">
-        <f>gstp*((1-gstp)^(G9-1))</f>
-        <v>7.9659417599999977E-2</v>
-      </c>
-      <c r="I9">
-        <f>I8+H9</f>
-        <v>0.58178805759999996</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J9">
+        <f t="shared" si="4"/>
+        <v>8.1381916800000023E-2</v>
+      </c>
+      <c r="K9">
+        <f>K8+J9</f>
+        <v>0.62926015680000014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>5</v>
       </c>
       <c r="B10">
-        <f>_xlfn.POISSON.DIST(A10,averageRaber,FALSE)</f>
-        <v>2.6028624134923937E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.13630319939969787</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>2.8623671873936551</v>
       </c>
       <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
         <v>5</v>
       </c>
-      <c r="E10">
-        <f>_xlfn.BINOM.DIST(A10,trials,stp,FALSE)</f>
+      <c r="F10">
+        <f t="shared" si="2"/>
         <v>1.0485759999999996E-4</v>
       </c>
       <c r="G10">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I10">
         <v>6</v>
       </c>
-      <c r="H10">
-        <f>gstp*((1-gstp)^(G10-1))</f>
-        <v>6.6913910783999983E-2</v>
-      </c>
-      <c r="I10">
-        <f>I9+H10</f>
-        <v>0.64870196838399996</v>
+      <c r="J10">
+        <f t="shared" si="4"/>
+        <v>6.6733171776000022E-2</v>
+      </c>
+      <c r="K10">
+        <f>K9+J10</f>
+        <v>0.69599332857600016</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>0.15361154758946899</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>3.2258424993788486</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>0.14838667024328117</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>3.1161200751089044</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>0.12542207093142427</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>2.6338634895599098</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>9.4232458726839122E-2</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>1.9788816332636217</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>6.371909338273074E-2</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>1.3381009610373455</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>3.9169314194559414E-2</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>0.82255559808574774</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>2.2071598458230215E-2</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>0.46350356762283451</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>1.148046553636148E-2</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>0.24108977626359107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>5.5449869509035755E-3</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>0.11644472596897508</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>2.4996449992166531E-3</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>5.2492544983549716E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>16</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>1.0563976261517556E-3</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>2.2184350149186866E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>4.2019178766256971E-4</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>8.8240275409139646E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>1.578498305530259E-4</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>3.3148464416135441E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>5.6177134656087314E-5</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>1.1797198277778336E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>20</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>1.8993222385833465E-5</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>3.9885767010250275E-4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DEA3D0B-EEBC-4570-8F64-EEFFE6192CD6}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>4695</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>5169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8">
+        <f>_xlfn.NORM.DIST(B6,B3,B4,TRUE)</f>
+        <v>0.8999174058669307</v>
+      </c>
+      <c r="C8">
+        <f>1-B8</f>
+        <v>0.1000825941330693</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8">
+        <f>_xlfn.NORM.INV(F3,B3,B4)</f>
+        <v>5169.174079251502</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C3A6F7-E52D-41FB-8111-9E210CC8F4BE}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>80</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8">
+        <f>_xlfn.NORM.DIST(B6,B3,B4,TRUE)</f>
+        <v>0.4012936743170763</v>
+      </c>
+      <c r="C8">
+        <f>1-B8</f>
+        <v>0.5987063256829237</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8">
+        <f>_xlfn.NORM.INV(F3,B3,B4)</f>
+        <v>105.63103131089201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9">
+        <f>_xlfn.NORM.DIST(90,B3,B4,TRUE)</f>
+        <v>0.69146246127401312</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14">
+        <f>B9-B8</f>
+        <v>0.29016878695693682</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Before Class Week 5
</commit_message>
<xml_diff>
--- a/data/ClassData.xlsx
+++ b/data/ClassData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\courses\qmsa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A71E40-9524-4C51-B4E7-E5587694DD9D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02E7D04-9858-4DCA-9370-6208C275A485}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="5" xr2:uid="{2FCD6EFA-A2DB-4D92-B665-54BD2494A43F}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="5" activeTab="6" xr2:uid="{2FCD6EFA-A2DB-4D92-B665-54BD2494A43F}"/>
   </bookViews>
   <sheets>
     <sheet name="3.1" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="DiscreateProbStarter" sheetId="4" r:id="rId4"/>
     <sheet name="ContinuousProbStarter" sheetId="6" r:id="rId5"/>
     <sheet name="ContinuousProbStarter (2)" sheetId="7" r:id="rId6"/>
+    <sheet name="RandomConfidence" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="averageRaber">DiscreateProbStarter!$B$3</definedName>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>Point</t>
   </si>
@@ -181,6 +182,33 @@
   </si>
   <si>
     <t>Answer(Cutoff)</t>
+  </si>
+  <si>
+    <t>Upper Bound</t>
+  </si>
+  <si>
+    <t>Lower Bound</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Outputs</t>
+  </si>
+  <si>
+    <t>Confidence</t>
+  </si>
+  <si>
+    <t>Samples</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>Worksheet for Random or Systematic Samples</t>
+  </si>
+  <si>
+    <t>PopStd</t>
   </si>
 </sst>
 </file>
@@ -1837,7 +1865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C3A6F7-E52D-41FB-8111-9E210CC8F4BE}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1919,4 +1947,102 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9015F821-CD3D-4794-9F44-22455BB07D22}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="15.578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1"/>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <f>_xlfn.CONFIDENCE.NORM((1-C7),C5,C6)</f>
+        <v>0.69785229220600398</v>
+      </c>
+      <c r="D10">
+        <f>C10*2</f>
+        <v>1.395704584412008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <f>C4-C10</f>
+        <v>8.9021477077939952</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12">
+        <f>C4+C10</f>
+        <v>10.297852292206004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>